<commit_message>
change the Ar volume to 28
</commit_message>
<xml_diff>
--- a/test_iso.xlsx
+++ b/test_iso.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="2_50" sheetId="1" r:id="rId1"/>
-    <sheet name="3_14" sheetId="2" r:id="rId2"/>
-    <sheet name="3_53" sheetId="3" r:id="rId3"/>
+    <sheet name="2_50_N2" sheetId="1" r:id="rId1"/>
+    <sheet name="3_14_N2" sheetId="2" r:id="rId2"/>
+    <sheet name="3_14_Ar" sheetId="4" r:id="rId3"/>
+    <sheet name="3_53_N2" sheetId="3" r:id="rId4"/>
+    <sheet name="1_223_kerogen_N2" sheetId="5" r:id="rId5"/>
+    <sheet name="1_223_kerogen_Ar" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="2">
   <si>
     <t>p_rels</t>
   </si>
@@ -656,10 +659,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,6 +677,213 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>0.30039199357601903</v>
+      </c>
+      <c r="B2">
+        <v>23.485313979899978</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.35157831214384816</v>
+      </c>
+      <c r="B3">
+        <v>25.096830687341605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.40083385408149758</v>
+      </c>
+      <c r="B4">
+        <v>26.654272914671349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.45023812996431944</v>
+      </c>
+      <c r="B5">
+        <v>28.328064345279635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.50017180111076964</v>
+      </c>
+      <c r="B6">
+        <v>30.063851833641163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.55050893566871761</v>
+      </c>
+      <c r="B7">
+        <v>31.971497841535967</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.60052934519391066</v>
+      </c>
+      <c r="B8">
+        <v>34.086843797606051</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.65035155363844099</v>
+      </c>
+      <c r="B9">
+        <v>36.530207219789425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.69967237242768132</v>
+      </c>
+      <c r="B10">
+        <v>39.372755128896202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.74970732790560368</v>
+      </c>
+      <c r="B11">
+        <v>42.820418167589622</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.79949086509117706</v>
+      </c>
+      <c r="B12">
+        <v>47.301878156506106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.82436493184885828</v>
+      </c>
+      <c r="B13">
+        <v>50.324152157731945</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.85020022918810589</v>
+      </c>
+      <c r="B14">
+        <v>53.963825289124699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.87422796715016959</v>
+      </c>
+      <c r="B15">
+        <v>58.176293881272059</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.89901568768798401</v>
+      </c>
+      <c r="B16">
+        <v>63.721176227716434</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.9230713909952859</v>
+      </c>
+      <c r="B17">
+        <v>71.004175191356225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.94648540550914972</v>
+      </c>
+      <c r="B18">
+        <v>81.629143906460556</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.95785726488730905</v>
+      </c>
+      <c r="B19">
+        <v>89.565133774591999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.96849475642195881</v>
+      </c>
+      <c r="B20">
+        <v>100.10731982164464</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.97758804409711664</v>
+      </c>
+      <c r="B21">
+        <v>113.56300189177291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.9860010623627754</v>
+      </c>
+      <c r="B22">
+        <v>134.30653303464081</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.9903985579994079</v>
+      </c>
+      <c r="B23">
+        <v>152.57754298777792</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.99347609632619271</v>
+      </c>
+      <c r="B24">
+        <v>169.6468955741785</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>0.30554898024114185</v>
       </c>
       <c r="B2">
@@ -790,6 +1000,556 @@
       </c>
       <c r="B16">
         <v>14.521108368585018</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.30119253839666976</v>
+      </c>
+      <c r="B2">
+        <v>43.520344870481068</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.35193313464421877</v>
+      </c>
+      <c r="B3">
+        <v>46.189840567168481</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.40016151218164148</v>
+      </c>
+      <c r="B4">
+        <v>48.724705505002504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.450009765625</v>
+      </c>
+      <c r="B5">
+        <v>51.47611203514024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.49952183894121072</v>
+      </c>
+      <c r="B6">
+        <v>54.393964482663613</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.54932484371947043</v>
+      </c>
+      <c r="B7">
+        <v>57.711395193162211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.59987771594002193</v>
+      </c>
+      <c r="B8">
+        <v>61.343723298054684</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.6132573854161304</v>
+      </c>
+      <c r="B9">
+        <v>62.539558439217842</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.62683866021608314</v>
+      </c>
+      <c r="B10">
+        <v>63.793438110225999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.64014058230669524</v>
+      </c>
+      <c r="B11">
+        <v>65.094393989811252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.65281551932676074</v>
+      </c>
+      <c r="B12">
+        <v>66.378532583145684</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.66623064879083416</v>
+      </c>
+      <c r="B13">
+        <v>67.762470191850198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.67855385122352663</v>
+      </c>
+      <c r="B14">
+        <v>69.156763250204108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.69186186939045646</v>
+      </c>
+      <c r="B15">
+        <v>70.568007301422512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.70480475512773422</v>
+      </c>
+      <c r="B16">
+        <v>72.008178716829818</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.71757888953986826</v>
+      </c>
+      <c r="B17">
+        <v>73.585128859709059</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.72921354495469559</v>
+      </c>
+      <c r="B18">
+        <v>75.019576425249994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.7409401958050934</v>
+      </c>
+      <c r="B19">
+        <v>76.530757086478957</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.75228916849994132</v>
+      </c>
+      <c r="B20">
+        <v>78.269147021443175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.76334982130392481</v>
+      </c>
+      <c r="B21">
+        <v>80.059175636229156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.77419236031243888</v>
+      </c>
+      <c r="B22">
+        <v>81.883503928365769</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.7851260478131955</v>
+      </c>
+      <c r="B23">
+        <v>83.816580574711182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.79605812346509619</v>
+      </c>
+      <c r="B24">
+        <v>85.708138105225331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.80634007773235239</v>
+      </c>
+      <c r="B25">
+        <v>87.890532543024307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.81664849632475134</v>
+      </c>
+      <c r="B26">
+        <v>90.057698662021082</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.8265550193224771</v>
+      </c>
+      <c r="B27">
+        <v>92.464762002472057</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.83636431184420357</v>
+      </c>
+      <c r="B28">
+        <v>94.839217638968705</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.84722632038814771</v>
+      </c>
+      <c r="B29">
+        <v>97.57794899358376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.85666529344358933</v>
+      </c>
+      <c r="B30">
+        <v>100.24158747798405</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.86569413865232725</v>
+      </c>
+      <c r="B31">
+        <v>103.21319750833669</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.87416809033559761</v>
+      </c>
+      <c r="B32">
+        <v>106.40969503453539</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.88334306853582556</v>
+      </c>
+      <c r="B33">
+        <v>109.69455746672806</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.89171370882645395</v>
+      </c>
+      <c r="B34">
+        <v>113.28470368738286</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.90012886877265474</v>
+      </c>
+      <c r="B35">
+        <v>117.3147693592414</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.97360841729458814</v>
+      </c>
+      <c r="B36">
+        <v>201.07762495135049</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0.97899290563827113</v>
+      </c>
+      <c r="B37">
+        <v>219.25214593472057</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0.98763923688181277</v>
+      </c>
+      <c r="B38">
+        <v>270.70623602418016</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0.99209903819206502</v>
+      </c>
+      <c r="B39">
+        <v>322.94745812676013</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.99265046495675524</v>
+      </c>
+      <c r="B40">
+        <v>331.09447803577751</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.30035589377417815</v>
+      </c>
+      <c r="B2">
+        <v>52.571591696904839</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.35194522049085075</v>
+      </c>
+      <c r="B3">
+        <v>56.279304316433425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.39969265288034533</v>
+      </c>
+      <c r="B4">
+        <v>59.739841141420207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.45012415919319165</v>
+      </c>
+      <c r="B5">
+        <v>63.488239313717379</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.49947729770145866</v>
+      </c>
+      <c r="B6">
+        <v>67.393691305711002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.54935387389567159</v>
+      </c>
+      <c r="B7">
+        <v>71.631260580204739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.59937364916865066</v>
+      </c>
+      <c r="B8">
+        <v>76.43755426948168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.64872423838742388</v>
+      </c>
+      <c r="B9">
+        <v>81.690630948754688</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.69797208521740228</v>
+      </c>
+      <c r="B10">
+        <v>87.975412368040367</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.74767131213207094</v>
+      </c>
+      <c r="B11">
+        <v>95.709974907273704</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.79700683760795576</v>
+      </c>
+      <c r="B12">
+        <v>105.70348102084671</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.82356379067037888</v>
+      </c>
+      <c r="B13">
+        <v>112.52051587474033</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.84858404237334506</v>
+      </c>
+      <c r="B14">
+        <v>120.56034663543336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.87250918518891762</v>
+      </c>
+      <c r="B15">
+        <v>130.07385737456764</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.8965256616526005</v>
+      </c>
+      <c r="B16">
+        <v>142.39983834985941</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.92084885224755175</v>
+      </c>
+      <c r="B17">
+        <v>158.87843884429617</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.94857153338927436</v>
+      </c>
+      <c r="B18">
+        <v>189.13090605152126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.95804263910360865</v>
+      </c>
+      <c r="B19">
+        <v>204.44244336656558</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.96661116187918417</v>
+      </c>
+      <c r="B20">
+        <v>224.4564731482709</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.97475835748665551</v>
+      </c>
+      <c r="B21">
+        <v>247.94420413181876</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.98423011514120828</v>
+      </c>
+      <c r="B22">
+        <v>291.91300217733379</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.98929717658768757</v>
+      </c>
+      <c r="B23">
+        <v>331.56311915239809</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.99120273467814202</v>
+      </c>
+      <c r="B24">
+        <v>349.61352603441293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.9922860705472033</v>
+      </c>
+      <c r="B25">
+        <v>367.46853766804099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>